<commit_message>
Fixed few bugs + finished work on --excel-output option + configured auto-addition to file extension and dynamic file finding
</commit_message>
<xml_diff>
--- a/sheets/mocksheet.xlsx
+++ b/sheets/mocksheet.xlsx
@@ -52,7 +52,7 @@
     <t>City</t>
   </si>
   <si>
-    <t>Vova</t>
+    <t>VovaVova123</t>
   </si>
   <si>
     <t>Vovovich</t>
@@ -469,7 +469,7 @@
     <col min="22" max="22" style="8" width="8.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +517,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -547,7 +547,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -571,7 +571,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -595,7 +595,7 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -619,7 +619,7 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -643,7 +643,7 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -667,7 +667,7 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -691,7 +691,7 @@
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -715,7 +715,7 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -739,7 +739,7 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -763,7 +763,7 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -787,7 +787,7 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -811,7 +811,7 @@
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -835,7 +835,7 @@
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -859,7 +859,7 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -883,7 +883,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -907,7 +907,7 @@
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -931,7 +931,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -955,7 +955,7 @@
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -979,7 +979,7 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1003,7 +1003,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1027,7 +1027,7 @@
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1051,7 +1051,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1075,7 +1075,7 @@
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1099,7 +1099,7 @@
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1123,7 +1123,7 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>

</xml_diff>